<commit_message>
Add individual place/account assignment to routes
- Add placeIds array to Route type for individual location assignments
- Add place assignment functions to RouteContext (addPlaceToRoute, removePlaceFromRoute, getPlaceRoute)
- Color markers by route when in Routes view mode
- Click-to-assign mode now works for both cities AND individual markers
- Show assigned places in sidebar route details with ability to remove
- Marker info window shows route assignment when clicked
- Route badge shows total count (cities + individual places)

This allows assigning individual accounts/locations to routes regardless
of which city they're in, enabling scenarios like adding Phoenix accounts
to a Scottsdale route.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/input/PAM 11-20-24 to 11-19-25.xlsx
+++ b/data/input/PAM 11-20-24 to 11-19-25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f43291edbdba4a3/Desktop/Fun Projects/sales_dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f43291edbdba4a3/Desktop/Fun Projects/sales_dashboard/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{C0AA7F63-4AF0-42C7-B1CE-C6332C02C862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25EC3C2B-8C19-4402-AED0-C2563DCB1CD2}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{C0AA7F63-4AF0-42C7-B1CE-C6332C02C862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85FC7F3C-14FC-47C5-8BC5-C3604CB96431}"/>
   <bookViews>
     <workbookView xWindow="30195" yWindow="1395" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$25:$AP$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$25:$AP$254</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1708,7 +1708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -13725,7 +13725,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A25:AP25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A25:AP254" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape"/>
   <headerFooter>

</xml_diff>